<commit_message>
LESSON 16 - RDBMS - B1 - Database Design - 16.03.2024
</commit_message>
<xml_diff>
--- a/Java21 QPhan Database Design.xlsx
+++ b/Java21 QPhan Database Design.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="B1. Mô hình quan hệ" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -18,9 +18,113 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="33">
+  <si>
+    <t>Product</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>ProductId</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>CategoryId</t>
+  </si>
+  <si>
+    <t>CategoryName</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Color</t>
+  </si>
+  <si>
+    <t>Material</t>
+  </si>
+  <si>
+    <t>NameUser</t>
+  </si>
+  <si>
+    <t>Address</t>
+  </si>
+  <si>
+    <t>PhoneNumber</t>
+  </si>
+  <si>
+    <t>PaymentType</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>OrderDate</t>
+  </si>
+  <si>
+    <t>TotalOfMoney</t>
+  </si>
+  <si>
+    <t>TransportFee</t>
+  </si>
+  <si>
+    <t>Uid</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>OrderStatus</t>
+  </si>
+  <si>
+    <t>StaffId</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>TotalSalesQuantity</t>
+  </si>
+  <si>
+    <t>InventoryNumber</t>
+  </si>
+  <si>
+    <t>TotalRevenue</t>
+  </si>
+  <si>
+    <t>Account</t>
+  </si>
+  <si>
+    <t>Role</t>
+  </si>
+  <si>
+    <t>Decribe</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +132,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +161,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -323,7 +457,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -331,12 +465,231 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C1:I51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="8" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" customWidth="1"/>
+    <col min="10" max="29" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="11" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="3:9" ht="24.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="18" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="19" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="21" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="22" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="36" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="37" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="38" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="39" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="40" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="43" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="44" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="45" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="48" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="49" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="24.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LESSON 16 - RDBMS - B2 - Database Design - 19.03.2024
</commit_message>
<xml_diff>
--- a/Java21 QPhan Database Design.xlsx
+++ b/Java21 QPhan Database Design.xlsx
@@ -1,13 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8283756-8373-4F29-A068-7BD6C3B4C55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -18,9 +24,280 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={0A2C71E2-FB65-453E-A0CE-DA68AC748C4F}</author>
+    <author>tc={DB6D448B-03BA-4B3A-BBF2-3890C3BF9252}</author>
+    <author>tc={A45CD628-6220-4A84-BFE6-08B4C0A79347}</author>
+    <author>tc={6D1B4555-C3EF-4466-A326-A7140030D108}</author>
+    <author>tc={62E11726-5009-4EEC-BAD0-5B3C7C1D5FAD}</author>
+    <author>tc={26B8D9B6-EB95-478B-9008-2D83A6E64F56}</author>
+    <author>tc={D83912D2-3198-4AAD-A2E8-506838B31F39}</author>
+  </authors>
+  <commentList>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{0A2C71E2-FB65-453E-A0CE-DA68AC748C4F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Không cần thuộc phòng ban, làm được mọi chức năng</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{DB6D448B-03BA-4B3A-BBF2-3890C3BF9252}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Có thể khác nhau khi khắc kích cỡ, màu sắc</t>
+      </text>
+    </comment>
+    <comment ref="H7" authorId="2" shapeId="0" xr:uid="{A45CD628-6220-4A84-BFE6-08B4C0A79347}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NhanVien, Quan Ly</t>
+      </text>
+    </comment>
+    <comment ref="B8" authorId="3" shapeId="0" xr:uid="{6D1B4555-C3EF-4466-A326-A7140030D108}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="E8" authorId="4" shapeId="0" xr:uid="{62E11726-5009-4EEC-BAD0-5B3C7C1D5FAD}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    MatHang - SoLuong</t>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="5" shapeId="0" xr:uid="{26B8D9B6-EB95-478B-9008-2D83A6E64F56}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tùy thuộc vào kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="E15" authorId="6" shapeId="0" xr:uid="{D83912D2-3198-4AAD-A2E8-506838B31F39}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+  <si>
+    <t>NhanVien</t>
+  </si>
+  <si>
+    <t>MaNV</t>
+  </si>
+  <si>
+    <t>DiaChi</t>
+  </si>
+  <si>
+    <t>KhachHang</t>
+  </si>
+  <si>
+    <t>MaKH</t>
+  </si>
+  <si>
+    <t>SoDienThoai</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Xác định các </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>đối tượng, thuộc tính</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> của đối tượng đó</t>
+    </r>
+  </si>
+  <si>
+    <t>MatHang</t>
+  </si>
+  <si>
+    <t>MaMH</t>
+  </si>
+  <si>
+    <t>GiaBan</t>
+  </si>
+  <si>
+    <t>GiaMua</t>
+  </si>
+  <si>
+    <t>LoaiHang</t>
+  </si>
+  <si>
+    <t>TenMH</t>
+  </si>
+  <si>
+    <t>SoLuong</t>
+  </si>
+  <si>
+    <t>MoTa</t>
+  </si>
+  <si>
+    <t>MoTa(opt)</t>
+  </si>
+  <si>
+    <t>HinhAnh(s)</t>
+  </si>
+  <si>
+    <t>MauSac(s)</t>
+  </si>
+  <si>
+    <t>TenLH</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>TenKH</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>TaiKhoan</t>
+  </si>
+  <si>
+    <t>MatKhau</t>
+  </si>
+  <si>
+    <t>DonHang</t>
+  </si>
+  <si>
+    <t>MaDH</t>
+  </si>
+  <si>
+    <t>NgayTaoDonHang</t>
+  </si>
+  <si>
+    <t>ChiTietMatHang</t>
+  </si>
+  <si>
+    <t>TongTien</t>
+  </si>
+  <si>
+    <t>PhiGiaoHang</t>
+  </si>
+  <si>
+    <t>PhuongThucThanhToan</t>
+  </si>
+  <si>
+    <t>DiaChiGiaoHang</t>
+  </si>
+  <si>
+    <t>SoDienThoaiGiaoHang</t>
+  </si>
+  <si>
+    <t>TrangThaiDonHang</t>
+  </si>
+  <si>
+    <t>NhanVienPhuTrach</t>
+  </si>
+  <si>
+    <t>KichCo(s), GioiTinh</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>SubItemGroup</t>
+  </si>
+  <si>
+    <t>ItemGroup</t>
+  </si>
+  <si>
+    <t>MaPTTT</t>
+  </si>
+  <si>
+    <t>MaTTDH</t>
+  </si>
+  <si>
+    <t>TenNV</t>
+  </si>
+  <si>
+    <t>ChucVu</t>
+  </si>
+  <si>
+    <t>MaCV</t>
+  </si>
+  <si>
+    <t>TenCV</t>
+  </si>
+  <si>
+    <t>STT</t>
+  </si>
+  <si>
+    <t>TuNgayNao</t>
+  </si>
+  <si>
+    <t>DenNgayNao</t>
+  </si>
+  <si>
+    <t>SoLuongBan</t>
+  </si>
+  <si>
+    <t>SoLuongTonKho</t>
+  </si>
+  <si>
+    <t>ThongKeMatHang</t>
+  </si>
+  <si>
+    <t>DoanhThuMatHang</t>
+  </si>
+  <si>
+    <t>ChiTietDonHang</t>
+  </si>
+  <si>
+    <t>SET NULL</t>
+  </si>
+  <si>
+    <t>CASCADE</t>
+  </si>
+  <si>
+    <t>NO ACTION = RESTRICT</t>
+  </si>
+  <si>
+    <t>DoanhThu</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +305,65 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFC000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -45,12 +371,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -66,6 +425,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Quyen Ngoc Phan" id="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" userId="S::Quyen.Ngoc.Phan@mgm-tp.com::a07336a7-4c4c-48f3-ae7a-f1af5b9df94c" providerId="AD"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -329,14 +694,443 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H4" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{0A2C71E2-FB65-453E-A0CE-DA68AC748C4F}">
+    <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2024-03-19T12:47:56.43" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{DB6D448B-03BA-4B3A-BBF2-3890C3BF9252}">
+    <text>Có thể khác nhau khi khắc kích cỡ, màu sắc</text>
+  </threadedComment>
+  <threadedComment ref="H7" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{A45CD628-6220-4A84-BFE6-08B4C0A79347}">
+    <text>NhanVien, Quan Ly</text>
+  </threadedComment>
+  <threadedComment ref="B8" dT="2024-03-19T12:47:34.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{6D1B4555-C3EF-4466-A326-A7140030D108}">
+    <text>Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="E8" dT="2024-03-19T13:03:25.80" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{62E11726-5009-4EEC-BAD0-5B3C7C1D5FAD}">
+    <text>MatHang - SoLuong</text>
+  </threadedComment>
+  <threadedComment ref="B11" dT="2024-03-19T12:50:20.23" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{26B8D9B6-EB95-478B-9008-2D83A6E64F56}">
+    <text>Tùy thuộc vào kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="E15" dT="2024-03-19T13:18:52.37" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{D83912D2-3198-4AAD-A2E8-506838B31F39}">
+    <text>Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="23" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="1" customWidth="1"/>
+    <col min="12" max="29" width="14.7109375" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+    </row>
+    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="25" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="26" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="33" s="1" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="34" s="1" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" s="1" customFormat="1" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
LESSSON 16 - RDBMS - B3 - Database Design - 30.03.2024
</commit_message>
<xml_diff>
--- a/Java21 QPhan Database Design.xlsx
+++ b/Java21 QPhan Database Design.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8283756-8373-4F29-A068-7BD6C3B4C55D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B02896-BEF2-41AD-95C7-0CE03572F58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29160" yWindow="585" windowWidth="28920" windowHeight="20130" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
+    <sheet name="B2. Mô hình logic" sheetId="2" r:id="rId2"/>
+    <sheet name="B3. Mô hình vật lý" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -96,8 +98,152 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={DE58EBA4-8560-490B-BAD4-3856E742A2AE}</author>
+    <author>tc={3771F8C7-5E16-455B-902B-DE716AF4612B}</author>
+    <author>tc={2DF7D111-0DDE-4E17-8E1D-16765C0D4B63}</author>
+    <author>tc={4C122E08-9A24-4E6F-AF60-D8CC5F67F5C9}</author>
+    <author>tc={F628BF43-B4A1-4CAB-9E74-2093B57EE48F}</author>
+    <author>tc={D99EB7D2-A530-4F60-83C2-B2B7CB02A0F3}</author>
+    <author>tc={6CA12232-A882-491A-914E-F23513B95950}</author>
+  </authors>
+  <commentList>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{DE58EBA4-8560-490B-BAD4-3856E742A2AE}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Không cần thuộc phòng ban, làm được mọi chức năng</t>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="1" shapeId="0" xr:uid="{3771F8C7-5E16-455B-902B-DE716AF4612B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Có thể khác nhau khi khắc kích cỡ, màu sắc</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="2" shapeId="0" xr:uid="{2DF7D111-0DDE-4E17-8E1D-16765C0D4B63}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="3" shapeId="0" xr:uid="{4C122E08-9A24-4E6F-AF60-D8CC5F67F5C9}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tùy thuộc vào kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="4" shapeId="0" xr:uid="{F628BF43-B4A1-4CAB-9E74-2093B57EE48F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</t>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="5" shapeId="0" xr:uid="{D99EB7D2-A530-4F60-83C2-B2B7CB02A0F3}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NhanVien, Quan Ly</t>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="6" shapeId="0" xr:uid="{6CA12232-A882-491A-914E-F23513B95950}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    MatHang - SoLuong</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={8EC58335-C900-492B-BA28-EE6A8C506FC5}</author>
+    <author>tc={1144A81F-624A-4B23-B595-9D1402E8D27F}</author>
+    <author>tc={1305DD5C-A913-487C-8B38-59BD0DFB2D0F}</author>
+    <author>tc={2EF56CA4-B381-4D19-AB55-279304C643C4}</author>
+    <author>tc={3E506E74-1462-46EA-BBC4-5332C354E78B}</author>
+    <author>tc={B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}</author>
+    <author>tc={56863EB2-C75F-4DC4-BC9B-96A37C741BB5}</author>
+  </authors>
+  <commentList>
+    <comment ref="H4" authorId="0" shapeId="0" xr:uid="{8EC58335-C900-492B-BA28-EE6A8C506FC5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Không cần thuộc phòng ban, làm được mọi chức năng</t>
+      </text>
+    </comment>
+    <comment ref="B6" authorId="1" shapeId="0" xr:uid="{1144A81F-624A-4B23-B595-9D1402E8D27F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Có thể khác nhau khi khắc kích cỡ, màu sắc</t>
+      </text>
+    </comment>
+    <comment ref="B7" authorId="2" shapeId="0" xr:uid="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="B9" authorId="3" shapeId="0" xr:uid="{2EF56CA4-B381-4D19-AB55-279304C643C4}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Tùy thuộc vào kích cỡ, màu sắc, chất liệu</t>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="4" shapeId="0" xr:uid="{3E506E74-1462-46EA-BBC4-5332C354E78B}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</t>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="5" shapeId="0" xr:uid="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    NhanVien, Quan Ly</t>
+      </text>
+    </comment>
+    <comment ref="E14" authorId="6" shapeId="0" xr:uid="{56863EB2-C75F-4DC4-BC9B-96A37C741BB5}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    MatHang - SoLuong</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="135">
   <si>
     <t>NhanVien</t>
   </si>
@@ -292,12 +438,251 @@
   <si>
     <t>DoanhThu</t>
   </si>
+  <si>
+    <t>Xác định lại các tập thực thể</t>
+  </si>
+  <si>
+    <t>Xác định lại các thuộc tính</t>
+  </si>
+  <si>
+    <t>Xác định khóa của mỗi tập thực thể</t>
+  </si>
+  <si>
+    <t>Xác định mối quan hệ giữa các tập thực thể</t>
+  </si>
+  <si>
+    <t>KichCo</t>
+  </si>
+  <si>
+    <t>MaKC</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>XXL</t>
+  </si>
+  <si>
+    <t>Mô tả(Chieu Cao, Can Nang)</t>
+  </si>
+  <si>
+    <t>….</t>
+  </si>
+  <si>
+    <t>GioiTinh</t>
+  </si>
+  <si>
+    <t>DoTuoiTuMay</t>
+  </si>
+  <si>
+    <t>DoTuoiDenMay</t>
+  </si>
+  <si>
+    <t>OOP</t>
+  </si>
+  <si>
+    <t>HAS-A IS-A</t>
+  </si>
+  <si>
+    <t>Item: ItemGroup</t>
+  </si>
+  <si>
+    <t>Item extends BaseItem</t>
+  </si>
+  <si>
+    <t>Item is-a BaseItem (thừa kế)</t>
+  </si>
+  <si>
+    <t>Item has ItemGroup(liên kết, kết hợp)</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>HAS-A</t>
+  </si>
+  <si>
+    <t>ThoiGianTaoDonHang</t>
+  </si>
+  <si>
+    <t>TrangThai</t>
+  </si>
+  <si>
+    <t>DH1</t>
+  </si>
+  <si>
+    <t>Da Dong Goi</t>
+  </si>
+  <si>
+    <t>Dang Giao</t>
+  </si>
+  <si>
+    <t>ThoiGian</t>
+  </si>
+  <si>
+    <t>NVPT</t>
+  </si>
+  <si>
+    <t>Le Van Teo</t>
+  </si>
+  <si>
+    <t>Hoang A</t>
+  </si>
+  <si>
+    <t>Xac Nhan Don Hang</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>PaymentMethod</t>
+  </si>
+  <si>
+    <t>OrderStatus</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>ItemStatistic</t>
+  </si>
+  <si>
+    <t>Revenue</t>
+  </si>
+  <si>
+    <t>Size</t>
+  </si>
+  <si>
+    <t>1. Xác định các bảng - TABLE</t>
+  </si>
+  <si>
+    <t>2. Xác định lại các thuộc tính - COLUMN NAME</t>
+  </si>
+  <si>
+    <t>--&gt; Tập thực thể(B2) --&gt; Table
+--&gt; Mối quan hệ(B2) --&gt; Table mới</t>
+  </si>
+  <si>
+    <t>--&gt; Thuộc tính(B2) -&gt; Column
+--&gt; Mối quan hệ(B2) -&gt; Column mới (khóa ngoại)</t>
+  </si>
+  <si>
+    <t>3. Xác định khóa chính (PRIMARY KEY) của từng TABLE</t>
+  </si>
+  <si>
+    <t>--&gt; Khoá(B2) --&gt; Chọn ra 1 khóa làm khóa chính để cài đặt phân biệt các dòng dữ liệu khác nhau trong 1 table</t>
+  </si>
+  <si>
+    <t>4. Xác định khóa ngoại (FOREIGN KEY) của từng TABLE</t>
+  </si>
+  <si>
+    <t>--&gt; Quan hệ 1-1 --&gt; Tạo khóa ngoại ở bảng bất kỳ liên kết đến khóa chính ở bảng còn lại
+--&gt; Lưu ý: khóa ngoại phải là duy nhất - UNIQUE</t>
+  </si>
+  <si>
+    <t>--&gt; Quan hệ 1-n --&gt; Tạo khóa ngoại bên bảng n(con) liên kết với khóa chính bên bảng 1(cha)
+--&gt; Lưu ý: khóa ngoại có thể trùng nhau để đảm bảo đúng dữ liệu 1-n</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> --&gt; Quan hệ n-n --&gt; Tạo bảng mới dùng để lưu trữ dữ liệu thể hiện quan hệ n-n
+--&gt; Lưu ý: bảng mới có ít nhất 2 columns là khóa ngoại liên kết đến từng bảng n-n, 2 columns đó cũng là khóa chính của bảng mới</t>
+  </si>
+  <si>
+    <t>===================================================================</t>
+  </si>
+  <si>
+    <t>Sau khi thiết kế xong cơ sở dữ liệu vật lý (giấy, bản vẽ, thiết kế) có 2 cách sau đây để tạo ra CSDL vật lý dùng trong coding</t>
+  </si>
+  <si>
+    <t>Cách 1: Sử dụng các tool vẽ ra database diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   + VD: Tool MySQL workbench, vẽ xong lưu lại ở file .mvb</t>
+  </si>
+  <si>
+    <t>Chạy file sql, thực thi tạo ra database cho mình</t>
+  </si>
+  <si>
+    <t>Cách 2: Sử dụng cú pháp SQL DDL(CREATE, ALTER, DROP database, column, table, constraints) để tạo database</t>
+  </si>
+  <si>
+    <t>Sau đó convert từ diagram sang code sql(tập lệnh create, alter, drop database table column ...) để tạo database, table, column, constraints(pk, fk, null, not null, unique ...)</t>
+  </si>
+  <si>
+    <t>--&gt; Nhanh lúc đầu, khó maintain về sau, hoàn toàn ko biết nước table đó tạo ra khi nào dùng làm chức năng gì code trong version nào</t>
+  </si>
+  <si>
+    <t>--&gt; Hơi mất thời gian lúc đầu tạo code sql, đảm bảo tính chính xác</t>
+  </si>
+  <si>
+    <t>--&gt; Sửa trực tiếp trên diagram ở local, code mình chạy được, dev khác ko chạy dc, dev khác ko biết mình sửa table, column nào</t>
+  </si>
+  <si>
+    <t>--&gt; Thêm sửa xóa thông tin gì liên quan đến database, lưu lại, chỉ cần push code lên, các dev còn lại lấy code chạy là ok</t>
+  </si>
+  <si>
+    <t>--&gt; Versioning</t>
+  </si>
+  <si>
+    <t>MaLH</t>
+  </si>
+  <si>
+    <t>T01_ITEM</t>
+  </si>
+  <si>
+    <t>T02_ITEMGROUP</t>
+  </si>
+  <si>
+    <t>T04_ITEM_DETAIL</t>
+  </si>
+  <si>
+    <t>C04_ITEM_ID</t>
+  </si>
+  <si>
+    <t>C04_SIZE_ID</t>
+  </si>
+  <si>
+    <t>SALES_PRICE</t>
+  </si>
+  <si>
+    <t>BUY_PRICE</t>
+  </si>
+  <si>
+    <t>AMOUNT</t>
+  </si>
+  <si>
+    <t>Forward Engineer</t>
+  </si>
+  <si>
+    <t>Diagram(mwb) --&gt; Code(sql)</t>
+  </si>
+  <si>
+    <t>Reverse Engineer</t>
+  </si>
+  <si>
+    <t>Code(sql) --&gt; Diagram(mwb)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -335,15 +720,53 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="12"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,7 +813,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -404,11 +827,47 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -720,12 +1179,64 @@
 </ThreadedComments>
 </file>
 
+<file path=xl/threadedComments/threadedComment2.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H4" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{DE58EBA4-8560-490B-BAD4-3856E742A2AE}">
+    <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
+  </threadedComment>
+  <threadedComment ref="B6" dT="2024-03-19T12:47:56.43" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3771F8C7-5E16-455B-902B-DE716AF4612B}">
+    <text>Có thể khác nhau khi khắc kích cỡ, màu sắc</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2024-03-19T12:47:34.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{2DF7D111-0DDE-4E17-8E1D-16765C0D4B63}">
+    <text>Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="B9" dT="2024-03-19T12:50:20.23" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{4C122E08-9A24-4E6F-AF60-D8CC5F67F5C9}">
+    <text>Tùy thuộc vào kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="E12" dT="2024-03-19T13:18:52.37" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{F628BF43-B4A1-4CAB-9E74-2093B57EE48F}">
+    <text>Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</text>
+  </threadedComment>
+  <threadedComment ref="H12" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{D99EB7D2-A530-4F60-83C2-B2B7CB02A0F3}">
+    <text>NhanVien, Quan Ly</text>
+  </threadedComment>
+  <threadedComment ref="E14" dT="2024-03-19T13:03:25.80" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{6CA12232-A882-491A-914E-F23513B95950}">
+    <text>MatHang - SoLuong</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
+<file path=xl/threadedComments/threadedComment3.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H4" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{8EC58335-C900-492B-BA28-EE6A8C506FC5}">
+    <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
+  </threadedComment>
+  <threadedComment ref="B6" dT="2024-03-19T12:47:56.43" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{1144A81F-624A-4B23-B595-9D1402E8D27F}">
+    <text>Có thể khác nhau khi khắc kích cỡ, màu sắc</text>
+  </threadedComment>
+  <threadedComment ref="B7" dT="2024-03-19T12:47:34.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
+    <text>Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="B9" dT="2024-03-19T12:50:20.23" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{2EF56CA4-B381-4D19-AB55-279304C643C4}">
+    <text>Tùy thuộc vào kích cỡ, màu sắc, chất liệu</text>
+  </threadedComment>
+  <threadedComment ref="E12" dT="2024-03-19T13:18:52.37" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3E506E74-1462-46EA-BBC4-5332C354E78B}">
+    <text>Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</text>
+  </threadedComment>
+  <threadedComment ref="H12" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
+    <text>NhanVien, Quan Ly</text>
+  </threadedComment>
+  <threadedComment ref="E14" dT="2024-03-19T13:03:25.80" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{56863EB2-C75F-4DC4-BC9B-96A37C741BB5}">
+    <text>MatHang - SoLuong</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -745,10 +1256,6 @@
   <sheetData>
     <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
@@ -1117,7 +1624,12 @@
       </c>
     </row>
     <row r="23" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="D24" s="6"/>
+    </row>
     <row r="25" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="26" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="27" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1133,4 +1645,1267 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B02AFA64-4F84-47ED-AB68-8CF3C6F7C8A6}">
+  <dimension ref="B1:L35"/>
+  <sheetViews>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="25.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="1" customWidth="1"/>
+    <col min="12" max="29" width="14.7109375" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H21" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J21" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="K21" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="G22" s="1">
+        <v>1</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" s="1">
+        <v>1</v>
+      </c>
+      <c r="J22" s="7">
+        <v>5</v>
+      </c>
+      <c r="K22" s="7">
+        <v>15</v>
+      </c>
+      <c r="L22" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G23" s="1">
+        <v>2</v>
+      </c>
+      <c r="H23" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" s="1">
+        <v>0</v>
+      </c>
+      <c r="J23" s="7">
+        <v>5</v>
+      </c>
+      <c r="K23" s="7">
+        <v>15</v>
+      </c>
+      <c r="L23" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G24" s="1">
+        <v>3</v>
+      </c>
+      <c r="H24" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="1">
+        <v>1</v>
+      </c>
+      <c r="J24" s="7">
+        <v>16</v>
+      </c>
+      <c r="K24" s="7">
+        <v>40</v>
+      </c>
+      <c r="L24" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="25" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="1">
+        <v>4</v>
+      </c>
+      <c r="H25" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="1">
+        <v>0</v>
+      </c>
+      <c r="J25" s="7">
+        <v>16</v>
+      </c>
+      <c r="K25" s="7">
+        <v>40</v>
+      </c>
+      <c r="L25" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H26" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="L26" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="27" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L27" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="28" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="29" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="H29" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="L29" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="30" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="31" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="32" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E32" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="G32" s="9">
+        <v>0.40972222222222221</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="33" spans="5:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E33" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F33" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="G33" s="9">
+        <v>0.41736111111111113</v>
+      </c>
+      <c r="H33" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="5:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="9">
+        <v>0.41805555555555557</v>
+      </c>
+      <c r="H34" s="1" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="5:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E744B-65C2-4DE9-994B-E5E54772E544}">
+  <dimension ref="B1:L52"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="33.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
+    <col min="8" max="9" width="14.7109375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="20" style="1" customWidth="1"/>
+    <col min="12" max="29" width="14.7109375" style="1" customWidth="1"/>
+    <col min="30" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+    </row>
+    <row r="3" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>94</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>96</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="K3" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="L3" s="6" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="5" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="K5" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="6" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="8" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="3"/>
+      <c r="D8" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+      <c r="H8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3"/>
+      <c r="J8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="14" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="21" spans="2:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
+      <c r="E21" s="11"/>
+      <c r="G21" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="I22" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="J22" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="K22" s="18" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="23" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="G23" s="1">
+        <v>11</v>
+      </c>
+      <c r="H23" s="1">
+        <v>1</v>
+      </c>
+      <c r="I23" s="1">
+        <v>220</v>
+      </c>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+    </row>
+    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="G24" s="1">
+        <v>11</v>
+      </c>
+      <c r="H24" s="1">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1">
+        <v>750</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
+    </row>
+    <row r="25" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="C25" s="13"/>
+      <c r="D25" s="13"/>
+      <c r="E25" s="13"/>
+      <c r="J25" s="7"/>
+      <c r="K25" s="7"/>
+    </row>
+    <row r="26" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="J26" s="7"/>
+      <c r="K26" s="7"/>
+    </row>
+    <row r="27" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11"/>
+      <c r="E27" s="11"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+    </row>
+    <row r="28" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="J28" s="7"/>
+      <c r="K28" s="7"/>
+    </row>
+    <row r="29" spans="2:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="C29" s="12"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+    </row>
+    <row r="30" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="15" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="17" t="s">
+        <v>112</v>
+      </c>
+      <c r="C34" s="16"/>
+      <c r="D34" s="16"/>
+    </row>
+    <row r="35" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G35" s="9"/>
+    </row>
+    <row r="36" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="G36" s="9"/>
+    </row>
+    <row r="37" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="G37" s="9"/>
+    </row>
+    <row r="38" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="15" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="39" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="40" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="C41" s="14"/>
+      <c r="D41" s="14"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="14"/>
+    </row>
+    <row r="42" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="43" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="44" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="15" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="45" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="48" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="52" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B21:E21"/>
+    <mergeCell ref="B23:E23"/>
+    <mergeCell ref="B25:E25"/>
+    <mergeCell ref="B27:E27"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B29:E29"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
LESSON 16 - RDBMS - B3 - Database Design - 30.03.2024
</commit_message>
<xml_diff>
--- a/Java21 QPhan Database Design.xlsx
+++ b/Java21 QPhan Database Design.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\qphan\Desktop\bkit\course - webapp\java21\3. Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B02896-BEF2-41AD-95C7-0CE03572F58C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94FFB83C-6E7A-45D7-B49E-184EC4146294}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29160" yWindow="585" windowWidth="28920" windowHeight="20130" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28920" yWindow="405" windowWidth="28815" windowHeight="20325" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="B1. Mô hình quan niệm" sheetId="1" r:id="rId1"/>
@@ -174,12 +174,15 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={8EC58335-C900-492B-BA28-EE6A8C506FC5}</author>
-    <author>tc={1144A81F-624A-4B23-B595-9D1402E8D27F}</author>
     <author>tc={1305DD5C-A913-487C-8B38-59BD0DFB2D0F}</author>
-    <author>tc={2EF56CA4-B381-4D19-AB55-279304C643C4}</author>
-    <author>tc={3E506E74-1462-46EA-BBC4-5332C354E78B}</author>
+    <author>tc={F01BC811-4E6C-4543-AA25-E955BE8491CD}</author>
+    <author>tc={3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}</author>
+    <author>tc={9527FEF5-CCFC-4F64-97A2-BBE2E29C2803}</author>
+    <author>tc={3DE62A8D-5F5B-409E-A562-B1F200B29412}</author>
+    <author>tc={43CCAF04-133F-49FE-87EB-557285BF8E90}</author>
+    <author>tc={2853FC81-A62F-4574-A1AA-7A29E9B44A89}</author>
     <author>tc={B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}</author>
-    <author>tc={56863EB2-C75F-4DC4-BC9B-96A37C741BB5}</author>
+    <author>tc={4B47AF2D-C770-4A5E-8158-147A119469B1}</author>
   </authors>
   <commentList>
     <comment ref="H4" authorId="0" shapeId="0" xr:uid="{8EC58335-C900-492B-BA28-EE6A8C506FC5}">
@@ -190,15 +193,7 @@
     Không cần thuộc phòng ban, làm được mọi chức năng</t>
       </text>
     </comment>
-    <comment ref="B6" authorId="1" shapeId="0" xr:uid="{1144A81F-624A-4B23-B595-9D1402E8D27F}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Có thể khác nhau khi khắc kích cỡ, màu sắc</t>
-      </text>
-    </comment>
-    <comment ref="B7" authorId="2" shapeId="0" xr:uid="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
+    <comment ref="B7" authorId="1" shapeId="0" xr:uid="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -206,23 +201,56 @@
     Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</t>
       </text>
     </comment>
-    <comment ref="B9" authorId="3" shapeId="0" xr:uid="{2EF56CA4-B381-4D19-AB55-279304C643C4}">
+    <comment ref="J8" authorId="2" shapeId="0" xr:uid="{F01BC811-4E6C-4543-AA25-E955BE8491CD}">
+      <text>
+        <t xml:space="preserve">[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Số lượng bán
+</t>
+      </text>
+    </comment>
+    <comment ref="M8" authorId="3" shapeId="0" xr:uid="{3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Tùy thuộc vào kích cỡ, màu sắc, chất liệu</t>
+    Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</t>
       </text>
     </comment>
-    <comment ref="E12" authorId="4" shapeId="0" xr:uid="{3E506E74-1462-46EA-BBC4-5332C354E78B}">
+    <comment ref="J9" authorId="4" shapeId="0" xr:uid="{9527FEF5-CCFC-4F64-97A2-BBE2E29C2803}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</t>
+    How - tính số lượng tồn kho theo giai đoạn ?</t>
       </text>
     </comment>
-    <comment ref="H12" authorId="5" shapeId="0" xr:uid="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
+    <comment ref="K9" authorId="5" shapeId="0" xr:uid="{3DE62A8D-5F5B-409E-A562-B1F200B29412}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Lưu thông tin bán những mặt hàng nào số lượng bao nhiêu, JSON, OBJECT</t>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="6" shapeId="0" xr:uid="{43CCAF04-133F-49FE-87EB-557285BF8E90}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Doanh thu cho mặt hàng theo giai đoạn</t>
+      </text>
+    </comment>
+    <comment ref="M10" authorId="7" shapeId="0" xr:uid="{2853FC81-A62F-4574-A1AA-7A29E9B44A89}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Số lượng hàng còn lại ở thời điểm hiện tại</t>
+      </text>
+    </comment>
+    <comment ref="H12" authorId="8" shapeId="0" xr:uid="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
@@ -230,12 +258,12 @@
     NhanVien, Quan Ly</t>
       </text>
     </comment>
-    <comment ref="E14" authorId="6" shapeId="0" xr:uid="{56863EB2-C75F-4DC4-BC9B-96A37C741BB5}">
+    <comment ref="I22" authorId="9" shapeId="0" xr:uid="{4B47AF2D-C770-4A5E-8158-147A119469B1}">
       <text>
         <t>[Threaded comment]
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
-    MatHang - SoLuong</t>
+    Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</t>
       </text>
     </comment>
   </commentList>
@@ -243,7 +271,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="228">
   <si>
     <t>NhanVien</t>
   </si>
@@ -639,33 +667,12 @@
     <t>--&gt; Versioning</t>
   </si>
   <si>
-    <t>MaLH</t>
-  </si>
-  <si>
     <t>T01_ITEM</t>
   </si>
   <si>
     <t>T02_ITEMGROUP</t>
   </si>
   <si>
-    <t>T04_ITEM_DETAIL</t>
-  </si>
-  <si>
-    <t>C04_ITEM_ID</t>
-  </si>
-  <si>
-    <t>C04_SIZE_ID</t>
-  </si>
-  <si>
-    <t>SALES_PRICE</t>
-  </si>
-  <si>
-    <t>BUY_PRICE</t>
-  </si>
-  <si>
-    <t>AMOUNT</t>
-  </si>
-  <si>
     <t>Forward Engineer</t>
   </si>
   <si>
@@ -676,13 +683,313 @@
   </si>
   <si>
     <t>Code(sql) --&gt; Diagram(mwb)</t>
+  </si>
+  <si>
+    <t>C01_ITEM_ID</t>
+  </si>
+  <si>
+    <t>C01_BUY_PRICE</t>
+  </si>
+  <si>
+    <t>C01_ITEM_NAME</t>
+  </si>
+  <si>
+    <t>T03_ORDER</t>
+  </si>
+  <si>
+    <t>T04_PAYMENT_METHOD</t>
+  </si>
+  <si>
+    <t>T05_ORDER_STATUS</t>
+  </si>
+  <si>
+    <t>T06_SIZE</t>
+  </si>
+  <si>
+    <t>T07_EMPLOYEE</t>
+  </si>
+  <si>
+    <t>T08_TITLE</t>
+  </si>
+  <si>
+    <t>T09_ITEM_STATISTIC</t>
+  </si>
+  <si>
+    <t>T10_REVENUE</t>
+  </si>
+  <si>
+    <t>T11_CUSTOMER</t>
+  </si>
+  <si>
+    <t>T12_ITEM_DETAIL</t>
+  </si>
+  <si>
+    <t>C12_ITEM_ID</t>
+  </si>
+  <si>
+    <t>C12_SALES_PRICE</t>
+  </si>
+  <si>
+    <t>C12_SIZE_ID</t>
+  </si>
+  <si>
+    <t>C12_COLOR</t>
+  </si>
+  <si>
+    <t>RED</t>
+  </si>
+  <si>
+    <t>GREEN</t>
+  </si>
+  <si>
+    <t>YELLOW</t>
+  </si>
+  <si>
+    <t>C12_AMOUNT</t>
+  </si>
+  <si>
+    <t>T13_GALLERY</t>
+  </si>
+  <si>
+    <t>C13_PATH</t>
+  </si>
+  <si>
+    <t>C13_ITEM_ID</t>
+  </si>
+  <si>
+    <t>C01_ITEM_GROUP_ID</t>
+  </si>
+  <si>
+    <t>C02_ITEMGROUP_ID</t>
+  </si>
+  <si>
+    <t>C02_ITEMGROUP_NAME</t>
+  </si>
+  <si>
+    <t>C03_ORDER_ID</t>
+  </si>
+  <si>
+    <t>C03_ORDER_TIME</t>
+  </si>
+  <si>
+    <t>C03_DELIVERY_FEE</t>
+  </si>
+  <si>
+    <t>C03_DELIVERY_ADDRESS</t>
+  </si>
+  <si>
+    <t>C03_RECEIVER_PHONE</t>
+  </si>
+  <si>
+    <t>C03_TOTAL_OF_MONEY</t>
+  </si>
+  <si>
+    <t>C04_PMETHOD_ID</t>
+  </si>
+  <si>
+    <t>C04_PMETHOD_DESC</t>
+  </si>
+  <si>
+    <t>C03_PMETHOD_ID</t>
+  </si>
+  <si>
+    <t>C03_CUSTOMER_ID</t>
+  </si>
+  <si>
+    <t>T14_ORDER_DETAIL</t>
+  </si>
+  <si>
+    <t>C14_ORDER_ID</t>
+  </si>
+  <si>
+    <t>C14_AMOUNT</t>
+  </si>
+  <si>
+    <t>C12_ITEM_DETAIL_ID</t>
+  </si>
+  <si>
+    <t>UNIQUE</t>
+  </si>
+  <si>
+    <t>C14_ITEM_DETAIL_ID</t>
+  </si>
+  <si>
+    <t>C05_ORDER_STATUS_ID</t>
+  </si>
+  <si>
+    <t>C05_ORDER_STATUS_DESC</t>
+  </si>
+  <si>
+    <t>T15_ORDER_STATUS_DETAIL</t>
+  </si>
+  <si>
+    <t>C15_ORDER_ID</t>
+  </si>
+  <si>
+    <t>C15_ORDER_STATUS_ID</t>
+  </si>
+  <si>
+    <t>C15_LAST_UPDATE</t>
+  </si>
+  <si>
+    <t>NV1</t>
+  </si>
+  <si>
+    <t>NV2</t>
+  </si>
+  <si>
+    <t>NV3</t>
+  </si>
+  <si>
+    <t>NV4</t>
+  </si>
+  <si>
+    <t>C15_EMPLOYEE_ID</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>NV7</t>
+  </si>
+  <si>
+    <t>Table ITEM_DETAIL là table được tạo ra từ quan hệ N-N của ITEM và SIZE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sau đó ITEM_DETAIL lại có quan hệ N-N với ORDER để tạo ra ORDER_DETAIL</t>
+  </si>
+  <si>
+    <t>Table ORDER_STATUS_DETAIL là table được tạo ra từ quan hệ N-N của ORDER và ORDER_STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sau đó ORDER_STATUS_DETAIL lại có quan hệ N-1 với EMPLOYEE, thêm khóa ngoại EMPLOYEE_ID vào ORDER_STATUS_DETAIL</t>
+  </si>
+  <si>
+    <t>C06_SIZE_ID</t>
+  </si>
+  <si>
+    <t>C06_SIZE_NAME</t>
+  </si>
+  <si>
+    <t>C06_GENDER</t>
+  </si>
+  <si>
+    <t>C06_SIZE_DESC</t>
+  </si>
+  <si>
+    <t>C07_EMPLOYEE_ID</t>
+  </si>
+  <si>
+    <t>C07_EMPLOYEE_NAME</t>
+  </si>
+  <si>
+    <t>C07_EMPLOYEE_ADDRESS</t>
+  </si>
+  <si>
+    <t>C07_EMPLOYEE_PHONE</t>
+  </si>
+  <si>
+    <t>C07_EMPLOYEE_EMAIL</t>
+  </si>
+  <si>
+    <t>C07_EMPLOYEE_USERNAME</t>
+  </si>
+  <si>
+    <t>C07_EMPLOYEE_PASSWORD</t>
+  </si>
+  <si>
+    <t>C07_TITLE_ID</t>
+  </si>
+  <si>
+    <t>C08_TITLE_ID</t>
+  </si>
+  <si>
+    <t>C08_TITLE_NAME</t>
+  </si>
+  <si>
+    <t>C09_ITEM_ID</t>
+  </si>
+  <si>
+    <t>C09_SALES_AMOUNT</t>
+  </si>
+  <si>
+    <t>C09_STOCK_AMOUNT</t>
+  </si>
+  <si>
+    <t>1/4/2024</t>
+  </si>
+  <si>
+    <t>Nhập vào 1000 mặt hàng Kẹo X1</t>
+  </si>
+  <si>
+    <t>Thống kê</t>
+  </si>
+  <si>
+    <t>20.04 - 22.04</t>
+  </si>
+  <si>
+    <t>C09_REVENUE</t>
+  </si>
+  <si>
+    <t>C09_DATE_UNITIL 23:59</t>
+  </si>
+  <si>
+    <t>C09_DATE_FROM 00:00</t>
+  </si>
+  <si>
+    <t>C10_RID</t>
+  </si>
+  <si>
+    <t>C10_DATE_FROM 00:00</t>
+  </si>
+  <si>
+    <t>C10_TOTAL_OF_MONEY</t>
+  </si>
+  <si>
+    <t>C10_DATE_UNITIL 23:59</t>
+  </si>
+  <si>
+    <t>--- Làm thêm</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_ID</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_NAME</t>
+  </si>
+  <si>
+    <t>C11_CUSTOMER_EMAIL</t>
+  </si>
+  <si>
+    <t>C11_EMPLOYEE_ADDRESS</t>
+  </si>
+  <si>
+    <t>C11_EMPLOYEE_PHONE</t>
+  </si>
+  <si>
+    <t>C11_EMPLOYEE_USERNAME</t>
+  </si>
+  <si>
+    <t>C11_EMPLOYEE_PASSWORD</t>
+  </si>
+  <si>
+    <t>Mô hình logic trên cơ sở đối tượng ==&gt; https://app.diagrams.net/#G1EC3kWNgwWJ-jrYKf-W24OTGjAV-pxvRf#%7B%22pageId%22%3A%22AbEYu_0bn73_d0lKOqK0%22%7D</t>
+  </si>
+  <si>
+    <t>Mô hình logic trên cơ sở mẫu tin ==&gt;</t>
+  </si>
+  <si>
+    <t>Có thể chỉnh sửa trong lúc tạo dữ liệu kiểm thử(test data) hoặc trong lúc làm bài tập, coding</t>
+  </si>
+  <si>
+    <t>Lưu ý: Bản cuối cùng tạm thời của phần thiết kế</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -704,12 +1011,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
     </font>
     <font>
       <b/>
@@ -771,8 +1072,61 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF92D050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -785,8 +1139,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -809,11 +1169,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -824,26 +1197,38 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -854,19 +1239,67 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1210,23 +1643,33 @@
   <threadedComment ref="H4" dT="2024-03-19T13:48:38.72" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{8EC58335-C900-492B-BA28-EE6A8C506FC5}">
     <text>Không cần thuộc phòng ban, làm được mọi chức năng</text>
   </threadedComment>
-  <threadedComment ref="B6" dT="2024-03-19T12:47:56.43" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{1144A81F-624A-4B23-B595-9D1402E8D27F}">
-    <text>Có thể khác nhau khi khắc kích cỡ, màu sắc</text>
-  </threadedComment>
   <threadedComment ref="B7" dT="2024-03-19T12:47:34.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{1305DD5C-A913-487C-8B38-59BD0DFB2D0F}">
     <text>Các sản phầm mua vào đều chung giá, k quan tâm kích cỡ, màu sắc, chất liệu</text>
   </threadedComment>
-  <threadedComment ref="B9" dT="2024-03-19T12:50:20.23" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{2EF56CA4-B381-4D19-AB55-279304C643C4}">
-    <text>Tùy thuộc vào kích cỡ, màu sắc, chất liệu</text>
+  <threadedComment ref="J8" dT="2024-04-02T13:49:52.63" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{F01BC811-4E6C-4543-AA25-E955BE8491CD}">
+    <text xml:space="preserve">Số lượng bán
+</text>
   </threadedComment>
-  <threadedComment ref="E12" dT="2024-03-19T13:18:52.37" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3E506E74-1462-46EA-BBC4-5332C354E78B}">
-    <text>Nhân Viên Của Cửa Hàng, mỗi nhân viên phụ trách 1/N trạng thái khác nhau</text>
+  <threadedComment ref="M8" dT="2024-04-02T12:50:53.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3702AC3F-ACCB-4FA5-81F8-3D4343E0ECEF}">
+    <text>Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</text>
+  </threadedComment>
+  <threadedComment ref="J9" dT="2024-04-02T13:53:56.18" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{9527FEF5-CCFC-4F64-97A2-BBE2E29C2803}">
+    <text>How - tính số lượng tồn kho theo giai đoạn ?</text>
+  </threadedComment>
+  <threadedComment ref="K9" dT="2024-04-02T14:04:54.01" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{3DE62A8D-5F5B-409E-A562-B1F200B29412}">
+    <text>Lưu thông tin bán những mặt hàng nào số lượng bao nhiêu, JSON, OBJECT</text>
+  </threadedComment>
+  <threadedComment ref="J10" dT="2024-04-02T13:55:15.51" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{43CCAF04-133F-49FE-87EB-557285BF8E90}">
+    <text>Doanh thu cho mặt hàng theo giai đoạn</text>
+  </threadedComment>
+  <threadedComment ref="M10" dT="2024-04-02T13:53:18.17" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{2853FC81-A62F-4574-A1AA-7A29E9B44A89}">
+    <text>Số lượng hàng còn lại ở thời điểm hiện tại</text>
   </threadedComment>
   <threadedComment ref="H12" dT="2024-03-19T13:49:56.69" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{B9E52DF8-6EBC-4DCF-8C8A-1994D6E5BB03}">
     <text>NhanVien, Quan Ly</text>
   </threadedComment>
-  <threadedComment ref="E14" dT="2024-03-19T13:03:25.80" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{56863EB2-C75F-4DC4-BC9B-96A37C741BB5}">
-    <text>MatHang - SoLuong</text>
+  <threadedComment ref="I22" dT="2024-04-02T12:50:53.71" personId="{B15EC451-E8A9-489D-8A37-9C829A4785F3}" id="{4B47AF2D-C770-4A5E-8158-147A119469B1}">
+    <text>Có rất nhiều màu sắc color, rgb, hexa -&gt; sử dụng varchar để lưu chứ k tạo 1 bảng riêng</text>
   </threadedComment>
 </ThreadedComments>
 </file>
@@ -1652,7 +2095,7 @@
   <dimension ref="B1:L35"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1670,9 +2113,15 @@
     <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
     <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6"/>
+      <c r="B2" s="1" t="s">
+        <v>225</v>
+      </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -2285,344 +2734,396 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{258E744B-65C2-4DE9-994B-E5E54772E544}">
-  <dimension ref="B1:L52"/>
+  <dimension ref="B1:P64"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E14"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="14.7109375" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="28.7109375" style="1" customWidth="1"/>
     <col min="5" max="5" width="33.28515625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="23.42578125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="19.140625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="14.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="19.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="20" style="1" customWidth="1"/>
-    <col min="12" max="29" width="14.7109375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="27.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" style="1" customWidth="1"/>
+    <col min="10" max="10" width="28.140625" style="1" customWidth="1"/>
+    <col min="11" max="11" width="27" style="1" customWidth="1"/>
+    <col min="12" max="12" width="30.5703125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="21.140625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="22.7109375" style="1" customWidth="1"/>
+    <col min="15" max="15" width="22.28515625" style="1" customWidth="1"/>
+    <col min="16" max="16" width="28.7109375" style="1" customWidth="1"/>
+    <col min="17" max="29" width="14.7109375" style="1" customWidth="1"/>
     <col min="30" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="6" t="s">
-        <v>124</v>
-      </c>
+    <row r="1" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
     </row>
-    <row r="3" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C3" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>92</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="H3" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>97</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="4" spans="2:12" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="6"/>
+      <c r="C3" s="6"/>
+      <c r="D3" s="6"/>
+      <c r="E3" s="6"/>
+      <c r="F3" s="6"/>
+      <c r="G3" s="6"/>
+      <c r="H3" s="6"/>
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="2:16" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>122</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>123</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>3</v>
+        <v>131</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>24</v>
+        <v>132</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>30</v>
+        <v>133</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>33</v>
+        <v>134</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>0</v>
+        <v>135</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>42</v>
+        <v>136</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>50</v>
+        <v>137</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>56</v>
+        <v>138</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="C5" s="8" t="s">
-        <v>122</v>
-      </c>
-      <c r="D5" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="F5" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="G5" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="I5" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J5" s="8" t="s">
-        <v>45</v>
+        <v>139</v>
+      </c>
+      <c r="M4" s="19" t="s">
+        <v>140</v>
+      </c>
+      <c r="N4" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="O4" s="31" t="s">
+        <v>165</v>
+      </c>
+      <c r="P4" s="19" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="D5" s="18" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="18" t="s">
+        <v>161</v>
+      </c>
+      <c r="F5" s="18" t="s">
+        <v>171</v>
+      </c>
+      <c r="G5" s="18" t="s">
+        <v>188</v>
+      </c>
+      <c r="H5" s="18" t="s">
+        <v>192</v>
+      </c>
+      <c r="I5" s="18" t="s">
+        <v>200</v>
+      </c>
+      <c r="J5" s="35" t="s">
+        <v>202</v>
       </c>
       <c r="K5" s="8" t="s">
-        <v>45</v>
+        <v>212</v>
       </c>
       <c r="L5" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>217</v>
+      </c>
+      <c r="M5" s="38" t="s">
+        <v>168</v>
+      </c>
+      <c r="N5" s="18" t="s">
+        <v>150</v>
+      </c>
+      <c r="O5" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="P5" s="18" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="6" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
-        <v>9</v>
+        <v>130</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>18</v>
+        <v>154</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>20</v>
+        <v>156</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>81</v>
+        <v>162</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>14</v>
+        <v>172</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>14</v>
+        <v>189</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>41</v>
+        <v>193</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>201</v>
+      </c>
+      <c r="J6" s="18" t="s">
+        <v>211</v>
+      </c>
+      <c r="K6" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="L6" s="8" t="s">
+        <v>218</v>
+      </c>
+      <c r="M6" s="25" t="s">
+        <v>141</v>
+      </c>
+      <c r="N6" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="O6" s="38" t="s">
+        <v>170</v>
+      </c>
+      <c r="P6" s="18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="7" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
-        <v>10</v>
+        <v>129</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>28</v>
-      </c>
+        <v>157</v>
+      </c>
+      <c r="E7" s="3"/>
       <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>190</v>
+      </c>
       <c r="H7" s="3" t="s">
-        <v>2</v>
+        <v>194</v>
       </c>
       <c r="I7" s="3"/>
-      <c r="J7" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7" s="3" t="s">
-        <v>47</v>
+      <c r="J7" s="18" t="s">
+        <v>210</v>
+      </c>
+      <c r="K7" s="18" t="s">
+        <v>215</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="8" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="3" t="s">
-        <v>12</v>
+        <v>219</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>143</v>
+      </c>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="8" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
+        <v>152</v>
       </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>29</v>
-      </c>
+        <v>158</v>
+      </c>
+      <c r="E8" s="3"/>
       <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>191</v>
+      </c>
       <c r="H8" s="3" t="s">
-        <v>5</v>
+        <v>195</v>
       </c>
       <c r="I8" s="3"/>
       <c r="J8" s="3" t="s">
-        <v>7</v>
+        <v>203</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>28</v>
+        <v>214</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="3" t="s">
-        <v>13</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="M8" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="9" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="4"/>
       <c r="C9" s="3"/>
       <c r="D9" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>31</v>
-      </c>
+        <v>159</v>
+      </c>
+      <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
       <c r="H9" s="3" t="s">
-        <v>21</v>
+        <v>196</v>
       </c>
       <c r="I9" s="3"/>
-      <c r="J9" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-    </row>
-    <row r="10" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="J9" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="K9" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+    </row>
+    <row r="10" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="4"/>
       <c r="C10" s="3"/>
       <c r="D10" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>32</v>
-      </c>
+        <v>160</v>
+      </c>
+      <c r="E10" s="3"/>
       <c r="F10" s="3"/>
       <c r="G10" s="3"/>
       <c r="H10" s="3" t="s">
-        <v>22</v>
+        <v>197</v>
       </c>
       <c r="I10" s="3"/>
       <c r="J10" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-    </row>
-    <row r="11" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="3" t="s">
-        <v>17</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="K10" s="37"/>
+      <c r="L10" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+    </row>
+    <row r="11" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="4"/>
       <c r="C11" s="3"/>
-      <c r="D11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>33</v>
-      </c>
+      <c r="D11" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>23</v>
+        <v>198</v>
       </c>
       <c r="I11" s="3"/>
-      <c r="J11" s="3" t="s">
-        <v>51</v>
-      </c>
+      <c r="J11" s="3"/>
       <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="4" t="s">
-        <v>61</v>
-      </c>
+      <c r="L11" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+    </row>
+    <row r="12" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="4"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="D12" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="4" t="s">
-        <v>42</v>
-      </c>
+        <v>199</v>
+      </c>
+      <c r="I12" s="36"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-    </row>
-    <row r="13" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="4" t="s">
-        <v>11</v>
-      </c>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+    </row>
+    <row r="13" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="3"/>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
-      <c r="E13" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="E13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
+      <c r="H13" s="36"/>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
-    </row>
-    <row r="14" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M13" s="3"/>
+      <c r="N13" s="3"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="3"/>
+    </row>
+    <row r="14" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
-      <c r="E14" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
       <c r="H14" s="3"/>
@@ -2630,26 +3131,32 @@
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
       <c r="L14" s="3"/>
-    </row>
-    <row r="15" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+    </row>
+    <row r="15" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
+      <c r="C15" s="36"/>
       <c r="D15" s="3"/>
-      <c r="E15" s="4" t="s">
-        <v>30</v>
-      </c>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-    </row>
-    <row r="16" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L15" s="36"/>
+      <c r="M15" s="3"/>
+      <c r="N15" s="3"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="3"/>
+    </row>
+    <row r="16" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="3"/>
       <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
+      <c r="D16" s="36"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
@@ -2658,8 +3165,12 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-    </row>
-    <row r="17" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+    </row>
+    <row r="17" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="3"/>
       <c r="C17" s="3"/>
       <c r="D17" s="3"/>
@@ -2671,8 +3182,12 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="M17" s="3"/>
+      <c r="N17" s="3"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="3"/>
+    </row>
+    <row r="18" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="3"/>
       <c r="C18" s="3"/>
       <c r="D18" s="3"/>
@@ -2684,226 +3199,424 @@
       <c r="J18" s="3"/>
       <c r="K18" s="3"/>
       <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="14" t="s">
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+    </row>
+    <row r="19" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="11" t="s">
         <v>100</v>
       </c>
-    </row>
-    <row r="21" spans="2:12" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="11" t="s">
+      <c r="K20" s="33" t="s">
+        <v>205</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="21" spans="2:16" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="C21" s="11"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="G21" s="1" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="22" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="14" t="s">
+      <c r="C21" s="15"/>
+      <c r="D21" s="15"/>
+      <c r="E21" s="15"/>
+      <c r="F21" s="22" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="24" t="s">
+        <v>169</v>
+      </c>
+      <c r="H21" s="24"/>
+      <c r="I21" s="24"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22" t="s">
+        <v>208</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="G22" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="H22" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="I22" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="J22" s="18" t="s">
-        <v>129</v>
-      </c>
-      <c r="K22" s="18" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="23" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="11" t="s">
+      <c r="F22" s="21" t="s">
+        <v>168</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>141</v>
+      </c>
+      <c r="H22" s="26" t="s">
+        <v>143</v>
+      </c>
+      <c r="I22" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="J22" s="22" t="s">
+        <v>142</v>
+      </c>
+      <c r="K22" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="G23" s="1">
+      <c r="C23" s="16"/>
+      <c r="D23" s="16"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="1">
+        <v>1</v>
+      </c>
+      <c r="G23" s="22">
         <v>11</v>
       </c>
-      <c r="H23" s="1">
+      <c r="H23" s="22">
         <v>1</v>
       </c>
-      <c r="I23" s="1">
+      <c r="I23" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="J23" s="23">
         <v>220</v>
       </c>
-      <c r="J23" s="7"/>
-      <c r="K23" s="7"/>
-    </row>
-    <row r="24" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="14" t="s">
+      <c r="K23" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="G24" s="1">
+      <c r="F24" s="1">
+        <v>2</v>
+      </c>
+      <c r="G24" s="22">
         <v>11</v>
       </c>
-      <c r="H24" s="1">
+      <c r="H24" s="22">
         <v>2</v>
       </c>
-      <c r="I24" s="1">
+      <c r="I24" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="J24" s="23">
         <v>750</v>
       </c>
-      <c r="J24" s="7"/>
-      <c r="K24" s="7"/>
-    </row>
-    <row r="25" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="11" t="s">
+      <c r="K24" s="23">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="C25" s="13"/>
-      <c r="D25" s="13"/>
-      <c r="E25" s="13"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="7"/>
-    </row>
-    <row r="26" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="14" t="s">
+      <c r="C25" s="17"/>
+      <c r="D25" s="17"/>
+      <c r="E25" s="17"/>
+      <c r="F25" s="1">
+        <v>3</v>
+      </c>
+      <c r="G25" s="22">
+        <v>11</v>
+      </c>
+      <c r="H25" s="22">
+        <v>1</v>
+      </c>
+      <c r="I25" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="J25" s="23">
+        <v>100</v>
+      </c>
+      <c r="K25" s="23">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="J26" s="7"/>
-      <c r="K26" s="7"/>
-    </row>
-    <row r="27" spans="2:12" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="11" t="s">
+      <c r="F26" s="1">
+        <v>4</v>
+      </c>
+      <c r="G26" s="27">
+        <v>11</v>
+      </c>
+      <c r="H26" s="27">
+        <v>1</v>
+      </c>
+      <c r="I26" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="J26" s="27">
+        <v>200</v>
+      </c>
+      <c r="K26" s="27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="2:16" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
+      <c r="C27" s="15"/>
+      <c r="D27" s="15"/>
+      <c r="E27" s="15"/>
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="2:12" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="11" t="s">
+    <row r="28" spans="2:16" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="C28" s="12"/>
-      <c r="D28" s="12"/>
-      <c r="E28" s="12"/>
+      <c r="C28" s="16"/>
+      <c r="D28" s="16"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="1" t="s">
+        <v>173</v>
+      </c>
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="2:12" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="11" t="s">
+    <row r="29" spans="2:16" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-    </row>
-    <row r="30" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:12" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="15" t="s">
+      <c r="C29" s="16"/>
+      <c r="D29" s="16"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="28" t="s">
+        <v>174</v>
+      </c>
+      <c r="G29" s="20" t="s">
+        <v>175</v>
+      </c>
+      <c r="H29" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="30" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F30" s="6">
+        <v>77</v>
+      </c>
+      <c r="G30" s="6">
+        <v>1</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="31" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F31" s="6">
+        <v>77</v>
+      </c>
+      <c r="G31" s="6">
+        <v>2</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="32" spans="2:16" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="12" t="s">
         <v>110</v>
       </c>
-    </row>
-    <row r="33" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F32" s="6">
+        <v>77</v>
+      </c>
+      <c r="G32" s="6">
+        <v>3</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="1" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="34" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B34" s="17" t="s">
+      <c r="F33" s="6">
+        <v>88</v>
+      </c>
+      <c r="G33" s="6">
+        <v>1</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C34" s="16"/>
-      <c r="D34" s="16"/>
-    </row>
-    <row r="35" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="F34" s="6">
+        <v>88</v>
+      </c>
+      <c r="G34" s="6">
+        <v>2</v>
+      </c>
+      <c r="H34" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B35" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="G35" s="9"/>
-    </row>
-    <row r="36" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F35" s="29">
+        <v>88</v>
+      </c>
+      <c r="G35" s="30" t="s">
+        <v>182</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="1" t="s">
         <v>116</v>
       </c>
       <c r="G36" s="9"/>
     </row>
-    <row r="37" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
         <v>114</v>
       </c>
       <c r="G37" s="9"/>
     </row>
-    <row r="38" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="15" t="s">
+    <row r="38" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="12" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="39" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="15" t="s">
+    <row r="39" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="40" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="14" t="s">
+    <row r="40" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="41" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="11" t="s">
         <v>115</v>
       </c>
-      <c r="C41" s="14"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="14"/>
-      <c r="F41" s="14"/>
-    </row>
-    <row r="42" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="15" t="s">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="11"/>
+      <c r="F41" s="11"/>
+    </row>
+    <row r="42" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="43" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="15" t="s">
+    <row r="43" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B43" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="44" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="15" t="s">
+    <row r="44" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="45" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="46" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="47" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B47" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="48" spans="2:7" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B48" s="1" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="49" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="50" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="51" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B51" s="13" t="s">
+        <v>184</v>
+      </c>
+      <c r="C51" s="13"/>
+      <c r="D51" s="13"/>
+      <c r="E51" s="13"/>
+      <c r="F51" s="13"/>
+    </row>
+    <row r="52" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B52" s="32" t="s">
+        <v>185</v>
+      </c>
+      <c r="C52" s="13"/>
+      <c r="D52" s="13"/>
+      <c r="E52" s="13"/>
+      <c r="F52" s="13"/>
+    </row>
+    <row r="53" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B53" s="13"/>
+      <c r="C53" s="13"/>
+      <c r="D53" s="13"/>
+      <c r="E53" s="13"/>
+      <c r="F53" s="13"/>
+    </row>
+    <row r="54" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B54" s="13"/>
+      <c r="C54" s="13"/>
+      <c r="D54" s="13"/>
+      <c r="E54" s="13"/>
+      <c r="F54" s="13"/>
+    </row>
+    <row r="55" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B55" s="13" t="s">
+        <v>186</v>
+      </c>
+      <c r="C55" s="13"/>
+      <c r="D55" s="13"/>
+      <c r="E55" s="13"/>
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B56" s="32" t="s">
+        <v>187</v>
+      </c>
+      <c r="C56" s="13"/>
+      <c r="D56" s="13"/>
+      <c r="E56" s="13"/>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="59" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="60" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="61" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="62" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="63" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="64" spans="2:6" ht="21.95" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B29:E29"/>
+    <mergeCell ref="G21:I21"/>
     <mergeCell ref="B21:E21"/>
     <mergeCell ref="B23:E23"/>
     <mergeCell ref="B25:E25"/>
     <mergeCell ref="B27:E27"/>
     <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B29:E29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>

</xml_diff>